<commit_message>
passage a openpyxl pour lire les excels
</commit_message>
<xml_diff>
--- a/Sondage.xlsx
+++ b/Sondage.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="343">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="397">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -1071,6 +1071,176 @@
   <x:si>
     <x:t xml:space="preserve">Optimisation des process et modes opératoires
 Amélioration de la cybersécurité</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Urbastyle SRL
+Fabrication de produits en béton architectonique</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Lanoy Jan</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">jan@urbastyle.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Wallonie</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Opinion de quelqu'un externe était très intéressant</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Pôle Mécatech</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">optimiser les postes de travail</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Techno Metal Industrie SPRL</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">C. Goffaux</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">goffaux.c@technometal.be</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">ERP</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Prise de conscience d'un plan de communication</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">société anonyme</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sandy Cognaux</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">sandy.cognaux@design-stone.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Expert, concept déjà couramment intégré dans les process de l’entreprise.</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Nous sommes dans le domaine de la pierre et déjà équipé d'un parc de machines numériques (robot, jet d'eau, débiteuse numérique, centre numérique 5 axes, ..)
+Cet accompagnement nous a permis de travailler sur l'organisation interne pour l'implémentation d'un programme ERP, et d'automatiser au maximum le travail au bureau et à l'atelier</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">voir point  10</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">au moins 3 actuellement et nous sommes encore à la recherche de personnel</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">?</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Fabrication de blocs cellulaires faits de paille, de chaux et d'eau pour construction de maisons. les avantages : légèreté et très isolant </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Olivier Beghin, administrateur délégué</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">o.b@isohemp.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">- programme d'évolution technologique et de rendement: séchage plus rapide des blocs
+- pilotage de l'unité</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">nouveaux équipements d'automatisation, nouvelle usine en projet, pilotage digital</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">augmentation d'emploi évident mais encore en augmentation en fonction des succès commerciaux </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">ergonomie et conditions de sécurité</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Réduction des coûts énergétiques.;Augmentation de la part des énergies vertes dans votre consommation d’énergie.;Réduction des consommables.;Réduction des rebuts/retouches/déchets.;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Domaine de la mécanique industrielle en mécano-soudure (conception et réalisation) - intervention aussi en maintenance et montage sur site</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Xavier Hellbois</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">xavier@erem.be</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">formation et premiers coaching de terrain (données, animation, plan digital)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">équipements de production
+ERP et différents modules
+réflexion pour une aide digitale</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">attention au COVID</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">implication et engagement de l'ensemble du personnel</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Réduction des coûts énergétiques.;Réduction des consommables.;Réduction des rebuts/retouches/déchets.;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Spécialiste dans l'installation de glissières de sécurité et dans l'équipement routier. Dispositifs performants alliant rigidité et ductilité </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">David Desaedeleer</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">david.desaedeleer@desami.be</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">10-15</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conception et réalisation d'équipements et matériel de confinement pour les sociétés pharmceutiques. Intervention dans les procédés de confinement et biodécontamination des salles blanches </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Michael Jeonty</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">m.jeonty@becarv.be</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">déjà compétent en système de pilotage des unités de biométhanisation
+intégration de tous les chapitres du 4.0 dans les limites de salles blanches </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Investissement en software et formation de compétences dans les divers chapitres de Factory 4.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">programme en développement et dans le COVID, pas évident de donner des chiffres - confiance pour le futur</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">conditions de travail et ergonomie</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Augmentation de la part des énergies vertes dans votre consommation d’énergie.;Réduction des rebuts/retouches/déchets.;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Design et fabrication de meubles spécialement pour chambre d'enfants
+artisans chevronnés travaillant avec des designers passionnés</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Jean-Marie Bols</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">mbb@mathy-by-bols.be</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Grâce aux contacts et experts, par exemple dans l'augmentation du CA (critique pour la société)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">machines adaptées à la découpe de bois et la peinture
+nouvelles opportunités en peinture </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">maintien et pérennisation  de l'emploi malgré le covid</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1167,8 +1337,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:CD40" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:CD40"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:CD48" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:CD48"/>
   <x:tableColumns count="82">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Heure de début" dataDxfId="3"/>
@@ -7080,11 +7250,1077 @@
       <x:c r="CC40"/>
       <x:c r="CD40" s="10" t="s"/>
     </x:row>
+    <x:row r="41" hidden="0">
+      <x:c r="A41">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B41" s="2">
+        <x:v>44165.5086342593</x:v>
+      </x:c>
+      <x:c r="C41" s="2">
+        <x:v>44165.6040277778</x:v>
+      </x:c>
+      <x:c r="D41" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E41" s="10" t="s"/>
+      <x:c r="F41"/>
+      <x:c r="G41" s="10" t="s"/>
+      <x:c r="H41" s="10" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="I41"/>
+      <x:c r="J41" s="10" t="s"/>
+      <x:c r="K41" s="10" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="L41"/>
+      <x:c r="M41" s="10" t="s"/>
+      <x:c r="N41" s="10" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="O41"/>
+      <x:c r="P41" s="10" t="s"/>
+      <x:c r="Q41" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R41"/>
+      <x:c r="S41" s="10" t="s"/>
+      <x:c r="T41" s="10" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="U41"/>
+      <x:c r="V41" s="10" t="s"/>
+      <x:c r="W41" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="X41"/>
+      <x:c r="Y41" s="10" t="s"/>
+      <x:c r="Z41" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="AA41"/>
+      <x:c r="AB41" s="10" t="s"/>
+      <x:c r="AC41" s="10" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="AD41"/>
+      <x:c r="AE41" s="10" t="s"/>
+      <x:c r="AF41" s="10" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="AG41"/>
+      <x:c r="AH41" s="10" t="s"/>
+      <x:c r="AI41" s="10" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="AJ41"/>
+      <x:c r="AK41" s="10" t="s"/>
+      <x:c r="AL41" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="AM41"/>
+      <x:c r="AN41" s="10" t="s"/>
+      <x:c r="AO41" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AP41"/>
+      <x:c r="AQ41" s="10" t="s"/>
+      <x:c r="AR41" s="10" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="AS41"/>
+      <x:c r="AT41" s="10" t="s"/>
+      <x:c r="AU41" s="10" t="s"/>
+      <x:c r="AV41"/>
+      <x:c r="AW41" s="10" t="s"/>
+      <x:c r="AX41" s="10" t="s"/>
+      <x:c r="AY41"/>
+      <x:c r="AZ41" s="10" t="s"/>
+      <x:c r="BA41" s="10" t="s"/>
+      <x:c r="BB41"/>
+      <x:c r="BC41" s="10" t="s"/>
+      <x:c r="BD41" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE41"/>
+      <x:c r="BF41" s="10" t="s"/>
+      <x:c r="BG41" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BH41"/>
+      <x:c r="BI41" s="10" t="s"/>
+      <x:c r="BJ41" s="10" t="s"/>
+      <x:c r="BK41"/>
+      <x:c r="BL41" s="10" t="s"/>
+      <x:c r="BM41" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BN41"/>
+      <x:c r="BO41" s="10" t="s"/>
+      <x:c r="BP41" s="10" t="s"/>
+      <x:c r="BQ41"/>
+      <x:c r="BR41" s="10" t="s"/>
+      <x:c r="BS41" s="10" t="s"/>
+      <x:c r="BT41"/>
+      <x:c r="BU41" s="10" t="s"/>
+      <x:c r="BV41" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BW41"/>
+      <x:c r="BX41" s="10" t="s"/>
+      <x:c r="BY41" s="10" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="BZ41"/>
+      <x:c r="CA41" s="10" t="s"/>
+      <x:c r="CB41" s="10" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="CC41"/>
+      <x:c r="CD41" s="10" t="s"/>
+    </x:row>
+    <x:row r="42" hidden="0">
+      <x:c r="A42">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B42" s="2">
+        <x:v>44165.6040625</x:v>
+      </x:c>
+      <x:c r="C42" s="2">
+        <x:v>44165.6059953704</x:v>
+      </x:c>
+      <x:c r="D42" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E42" s="10" t="s"/>
+      <x:c r="F42"/>
+      <x:c r="G42" s="10" t="s"/>
+      <x:c r="H42" s="10" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="I42"/>
+      <x:c r="J42" s="10" t="s"/>
+      <x:c r="K42" s="10" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="L42"/>
+      <x:c r="M42" s="10" t="s"/>
+      <x:c r="N42" s="10" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="O42"/>
+      <x:c r="P42" s="10" t="s"/>
+      <x:c r="Q42" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R42"/>
+      <x:c r="S42" s="10" t="s"/>
+      <x:c r="T42" s="10" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="U42"/>
+      <x:c r="V42" s="10" t="s"/>
+      <x:c r="W42" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="X42"/>
+      <x:c r="Y42" s="10" t="s"/>
+      <x:c r="Z42" s="10" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="AA42"/>
+      <x:c r="AB42" s="10" t="s"/>
+      <x:c r="AC42" s="10" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="AD42"/>
+      <x:c r="AE42" s="10" t="s"/>
+      <x:c r="AF42" s="10" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="AG42"/>
+      <x:c r="AH42" s="10" t="s"/>
+      <x:c r="AI42" s="10" t="s"/>
+      <x:c r="AJ42"/>
+      <x:c r="AK42" s="10" t="s"/>
+      <x:c r="AL42" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="AM42"/>
+      <x:c r="AN42" s="10" t="s"/>
+      <x:c r="AO42" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AP42"/>
+      <x:c r="AQ42" s="10" t="s"/>
+      <x:c r="AR42" s="10" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="AS42"/>
+      <x:c r="AT42" s="10" t="s"/>
+      <x:c r="AU42" s="10" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="AV42"/>
+      <x:c r="AW42" s="10" t="s"/>
+      <x:c r="AX42" s="10" t="s"/>
+      <x:c r="AY42"/>
+      <x:c r="AZ42" s="10" t="s"/>
+      <x:c r="BA42" s="10" t="s"/>
+      <x:c r="BB42"/>
+      <x:c r="BC42" s="10" t="s"/>
+      <x:c r="BD42" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE42"/>
+      <x:c r="BF42" s="10" t="s"/>
+      <x:c r="BG42" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BH42"/>
+      <x:c r="BI42" s="10" t="s"/>
+      <x:c r="BJ42" s="10" t="s"/>
+      <x:c r="BK42"/>
+      <x:c r="BL42" s="10" t="s"/>
+      <x:c r="BM42" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BN42"/>
+      <x:c r="BO42" s="10" t="s"/>
+      <x:c r="BP42" s="10" t="s"/>
+      <x:c r="BQ42"/>
+      <x:c r="BR42" s="10" t="s"/>
+      <x:c r="BS42" s="10" t="s"/>
+      <x:c r="BT42"/>
+      <x:c r="BU42" s="10" t="s"/>
+      <x:c r="BV42" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BW42"/>
+      <x:c r="BX42" s="10" t="s"/>
+      <x:c r="BY42" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="BZ42"/>
+      <x:c r="CA42" s="10" t="s"/>
+      <x:c r="CB42" s="10" t="s"/>
+      <x:c r="CC42"/>
+      <x:c r="CD42" s="10" t="s"/>
+    </x:row>
+    <x:row r="43" hidden="0">
+      <x:c r="A43">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B43" s="2">
+        <x:v>44173.6961689815</x:v>
+      </x:c>
+      <x:c r="C43" s="2">
+        <x:v>44173.6997453704</x:v>
+      </x:c>
+      <x:c r="D43" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E43" s="10" t="s"/>
+      <x:c r="F43"/>
+      <x:c r="G43" s="10" t="s"/>
+      <x:c r="H43" s="10" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="I43"/>
+      <x:c r="J43" s="10" t="s"/>
+      <x:c r="K43" s="10" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="L43"/>
+      <x:c r="M43" s="10" t="s"/>
+      <x:c r="N43" s="10" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="O43"/>
+      <x:c r="P43" s="10" t="s"/>
+      <x:c r="Q43" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R43"/>
+      <x:c r="S43" s="10" t="s"/>
+      <x:c r="T43" s="10" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="U43"/>
+      <x:c r="V43" s="10" t="s"/>
+      <x:c r="W43" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="X43"/>
+      <x:c r="Y43" s="10" t="s"/>
+      <x:c r="Z43" s="10" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="AA43"/>
+      <x:c r="AB43" s="10" t="s"/>
+      <x:c r="AC43" s="10" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="AD43"/>
+      <x:c r="AE43" s="10" t="s"/>
+      <x:c r="AF43" s="10" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="AG43"/>
+      <x:c r="AH43" s="10" t="s"/>
+      <x:c r="AI43" s="10" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="AJ43"/>
+      <x:c r="AK43" s="10" t="s"/>
+      <x:c r="AL43" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="AM43"/>
+      <x:c r="AN43" s="10" t="s"/>
+      <x:c r="AO43" s="10" t="s"/>
+      <x:c r="AP43"/>
+      <x:c r="AQ43" s="10" t="s"/>
+      <x:c r="AR43" s="10" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="AS43"/>
+      <x:c r="AT43" s="10" t="s"/>
+      <x:c r="AU43" s="10" t="s"/>
+      <x:c r="AV43"/>
+      <x:c r="AW43" s="10" t="s"/>
+      <x:c r="AX43" s="10" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="AY43"/>
+      <x:c r="AZ43" s="10" t="s"/>
+      <x:c r="BA43" s="10" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="BB43"/>
+      <x:c r="BC43" s="10" t="s"/>
+      <x:c r="BD43" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE43"/>
+      <x:c r="BF43" s="10" t="s"/>
+      <x:c r="BG43" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BH43"/>
+      <x:c r="BI43" s="10" t="s"/>
+      <x:c r="BJ43" s="10" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="BK43"/>
+      <x:c r="BL43" s="10" t="s"/>
+      <x:c r="BM43" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BN43"/>
+      <x:c r="BO43" s="10" t="s"/>
+      <x:c r="BP43" s="10" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="BQ43"/>
+      <x:c r="BR43" s="10" t="s"/>
+      <x:c r="BS43" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BT43"/>
+      <x:c r="BU43" s="10" t="s"/>
+      <x:c r="BV43" s="10" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="BW43"/>
+      <x:c r="BX43" s="10" t="s"/>
+      <x:c r="BY43" s="10" t="s"/>
+      <x:c r="BZ43"/>
+      <x:c r="CA43" s="10" t="s"/>
+      <x:c r="CB43" s="10" t="s"/>
+      <x:c r="CC43"/>
+      <x:c r="CD43" s="10" t="s"/>
+    </x:row>
+    <x:row r="44" hidden="0">
+      <x:c r="A44">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B44" s="2">
+        <x:v>44173.6998032407</x:v>
+      </x:c>
+      <x:c r="C44" s="2">
+        <x:v>44173.7033449074</x:v>
+      </x:c>
+      <x:c r="D44" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E44" s="10" t="s"/>
+      <x:c r="F44"/>
+      <x:c r="G44" s="10" t="s"/>
+      <x:c r="H44" s="10" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="I44"/>
+      <x:c r="J44" s="10" t="s"/>
+      <x:c r="K44" s="10" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="L44"/>
+      <x:c r="M44" s="10" t="s"/>
+      <x:c r="N44" s="10" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="O44"/>
+      <x:c r="P44" s="10" t="s"/>
+      <x:c r="Q44" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R44"/>
+      <x:c r="S44" s="10" t="s"/>
+      <x:c r="T44" s="10" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="U44"/>
+      <x:c r="V44" s="10" t="s"/>
+      <x:c r="W44" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="X44"/>
+      <x:c r="Y44" s="10" t="s"/>
+      <x:c r="Z44" s="10" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="AA44"/>
+      <x:c r="AB44" s="10" t="s"/>
+      <x:c r="AC44" s="10" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="AD44"/>
+      <x:c r="AE44" s="10" t="s"/>
+      <x:c r="AF44" s="10" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="AG44"/>
+      <x:c r="AH44" s="10" t="s"/>
+      <x:c r="AI44" s="10" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="AJ44"/>
+      <x:c r="AK44" s="10" t="s"/>
+      <x:c r="AL44" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="AM44"/>
+      <x:c r="AN44" s="10" t="s"/>
+      <x:c r="AO44" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AP44"/>
+      <x:c r="AQ44" s="10" t="s"/>
+      <x:c r="AR44" s="10" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="AS44"/>
+      <x:c r="AT44" s="10" t="s"/>
+      <x:c r="AU44" s="10" t="s"/>
+      <x:c r="AV44"/>
+      <x:c r="AW44" s="10" t="s"/>
+      <x:c r="AX44" s="10" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="AY44"/>
+      <x:c r="AZ44" s="10" t="s"/>
+      <x:c r="BA44" s="10" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="BB44"/>
+      <x:c r="BC44" s="10" t="s"/>
+      <x:c r="BD44" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE44"/>
+      <x:c r="BF44" s="10" t="s"/>
+      <x:c r="BG44" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BH44"/>
+      <x:c r="BI44" s="10" t="s"/>
+      <x:c r="BJ44" s="10" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="BK44"/>
+      <x:c r="BL44" s="10" t="s"/>
+      <x:c r="BM44" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BN44"/>
+      <x:c r="BO44" s="10" t="s"/>
+      <x:c r="BP44" s="7" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="BQ44"/>
+      <x:c r="BR44" s="10" t="s"/>
+      <x:c r="BS44" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BT44"/>
+      <x:c r="BU44" s="10" t="s"/>
+      <x:c r="BV44" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BW44"/>
+      <x:c r="BX44" s="10" t="s"/>
+      <x:c r="BY44" s="10" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="BZ44"/>
+      <x:c r="CA44" s="10" t="s"/>
+      <x:c r="CB44" s="10" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="CC44"/>
+      <x:c r="CD44" s="10" t="s"/>
+    </x:row>
+    <x:row r="45" hidden="0">
+      <x:c r="A45">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B45" s="2">
+        <x:v>44173.7034027778</x:v>
+      </x:c>
+      <x:c r="C45" s="2">
+        <x:v>44173.7065740741</x:v>
+      </x:c>
+      <x:c r="D45" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E45" s="10" t="s"/>
+      <x:c r="F45"/>
+      <x:c r="G45" s="10" t="s"/>
+      <x:c r="H45" s="10" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="I45"/>
+      <x:c r="J45" s="10" t="s"/>
+      <x:c r="K45" s="10" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="L45"/>
+      <x:c r="M45" s="10" t="s"/>
+      <x:c r="N45" s="10" t="s">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="O45"/>
+      <x:c r="P45" s="10" t="s"/>
+      <x:c r="Q45" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R45"/>
+      <x:c r="S45" s="10" t="s"/>
+      <x:c r="T45" s="10" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="U45"/>
+      <x:c r="V45" s="10" t="s"/>
+      <x:c r="W45" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="X45"/>
+      <x:c r="Y45" s="10" t="s"/>
+      <x:c r="Z45" s="10" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="AA45"/>
+      <x:c r="AB45" s="10" t="s"/>
+      <x:c r="AC45" s="10" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="AD45"/>
+      <x:c r="AE45" s="10" t="s"/>
+      <x:c r="AF45" s="10" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="AG45"/>
+      <x:c r="AH45" s="10" t="s"/>
+      <x:c r="AI45" s="10" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="AJ45"/>
+      <x:c r="AK45" s="10" t="s"/>
+      <x:c r="AL45" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="AM45"/>
+      <x:c r="AN45" s="10" t="s"/>
+      <x:c r="AO45" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AP45"/>
+      <x:c r="AQ45" s="10" t="s"/>
+      <x:c r="AR45" s="10" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="AS45"/>
+      <x:c r="AT45" s="10" t="s"/>
+      <x:c r="AU45" s="10" t="s"/>
+      <x:c r="AV45"/>
+      <x:c r="AW45" s="10" t="s"/>
+      <x:c r="AX45" s="10" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="AY45"/>
+      <x:c r="AZ45" s="10" t="s"/>
+      <x:c r="BA45" s="10" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="BB45"/>
+      <x:c r="BC45" s="10" t="s"/>
+      <x:c r="BD45" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE45"/>
+      <x:c r="BF45" s="10" t="s"/>
+      <x:c r="BG45" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BH45"/>
+      <x:c r="BI45" s="10" t="s"/>
+      <x:c r="BJ45" s="10" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="BK45"/>
+      <x:c r="BL45" s="10" t="s"/>
+      <x:c r="BM45" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BN45"/>
+      <x:c r="BO45" s="10" t="s"/>
+      <x:c r="BP45" s="10" t="s"/>
+      <x:c r="BQ45"/>
+      <x:c r="BR45" s="10" t="s"/>
+      <x:c r="BS45" s="10" t="s"/>
+      <x:c r="BT45"/>
+      <x:c r="BU45" s="10" t="s"/>
+      <x:c r="BV45" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BW45"/>
+      <x:c r="BX45" s="10" t="s"/>
+      <x:c r="BY45" s="10" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="BZ45"/>
+      <x:c r="CA45" s="10" t="s"/>
+      <x:c r="CB45" s="10" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="CC45"/>
+      <x:c r="CD45" s="10" t="s"/>
+    </x:row>
+    <x:row r="46" hidden="0">
+      <x:c r="A46">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B46" s="2">
+        <x:v>44174.3453125</x:v>
+      </x:c>
+      <x:c r="C46" s="2">
+        <x:v>44174.347662037</x:v>
+      </x:c>
+      <x:c r="D46" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E46" s="10" t="s"/>
+      <x:c r="F46"/>
+      <x:c r="G46" s="10" t="s"/>
+      <x:c r="H46" s="10" t="s">
+        <x:v>379</x:v>
+      </x:c>
+      <x:c r="I46"/>
+      <x:c r="J46" s="10" t="s"/>
+      <x:c r="K46" s="10" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="L46"/>
+      <x:c r="M46" s="10" t="s"/>
+      <x:c r="N46" s="10" t="s">
+        <x:v>381</x:v>
+      </x:c>
+      <x:c r="O46"/>
+      <x:c r="P46" s="10" t="s"/>
+      <x:c r="Q46" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R46"/>
+      <x:c r="S46" s="10" t="s"/>
+      <x:c r="T46" s="10" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="U46"/>
+      <x:c r="V46" s="10" t="s"/>
+      <x:c r="W46" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="X46"/>
+      <x:c r="Y46" s="10" t="s"/>
+      <x:c r="Z46" s="10" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="AA46"/>
+      <x:c r="AB46" s="10" t="s"/>
+      <x:c r="AC46" s="10" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="AD46"/>
+      <x:c r="AE46" s="10" t="s"/>
+      <x:c r="AF46" s="10" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="AG46"/>
+      <x:c r="AH46" s="10" t="s"/>
+      <x:c r="AI46" s="10" t="s"/>
+      <x:c r="AJ46"/>
+      <x:c r="AK46" s="10" t="s"/>
+      <x:c r="AL46" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="AM46"/>
+      <x:c r="AN46" s="10" t="s"/>
+      <x:c r="AO46" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AP46"/>
+      <x:c r="AQ46" s="10" t="s"/>
+      <x:c r="AR46" s="10" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="AS46"/>
+      <x:c r="AT46" s="10" t="s"/>
+      <x:c r="AU46" s="10" t="s"/>
+      <x:c r="AV46"/>
+      <x:c r="AW46" s="10" t="s"/>
+      <x:c r="AX46" s="10" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="AY46"/>
+      <x:c r="AZ46" s="10" t="s"/>
+      <x:c r="BA46" s="10" t="s"/>
+      <x:c r="BB46"/>
+      <x:c r="BC46" s="10" t="s"/>
+      <x:c r="BD46" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE46"/>
+      <x:c r="BF46" s="10" t="s"/>
+      <x:c r="BG46" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BH46"/>
+      <x:c r="BI46" s="10" t="s"/>
+      <x:c r="BJ46" s="10" t="s"/>
+      <x:c r="BK46"/>
+      <x:c r="BL46" s="10" t="s"/>
+      <x:c r="BM46" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BN46"/>
+      <x:c r="BO46" s="10" t="s"/>
+      <x:c r="BP46" s="10" t="s">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="BQ46"/>
+      <x:c r="BR46" s="10" t="s"/>
+      <x:c r="BS46" s="10" t="s"/>
+      <x:c r="BT46"/>
+      <x:c r="BU46" s="10" t="s"/>
+      <x:c r="BV46" s="10" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="BW46"/>
+      <x:c r="BX46" s="10" t="s"/>
+      <x:c r="BY46" s="10" t="s"/>
+      <x:c r="BZ46"/>
+      <x:c r="CA46" s="10" t="s"/>
+      <x:c r="CB46" s="10" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="CC46"/>
+      <x:c r="CD46" s="10" t="s"/>
+    </x:row>
+    <x:row r="47" hidden="0">
+      <x:c r="A47">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B47" s="2">
+        <x:v>44174.3477199074</x:v>
+      </x:c>
+      <x:c r="C47" s="2">
+        <x:v>44174.3515972222</x:v>
+      </x:c>
+      <x:c r="D47" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E47" s="10" t="s"/>
+      <x:c r="F47"/>
+      <x:c r="G47" s="10" t="s"/>
+      <x:c r="H47" s="10" t="s">
+        <x:v>383</x:v>
+      </x:c>
+      <x:c r="I47"/>
+      <x:c r="J47" s="10" t="s"/>
+      <x:c r="K47" s="10" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="L47"/>
+      <x:c r="M47" s="10" t="s"/>
+      <x:c r="N47" s="10" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="O47"/>
+      <x:c r="P47" s="10" t="s"/>
+      <x:c r="Q47" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R47"/>
+      <x:c r="S47" s="10" t="s"/>
+      <x:c r="T47" s="10" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="U47"/>
+      <x:c r="V47" s="10" t="s"/>
+      <x:c r="W47" s="10" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="X47"/>
+      <x:c r="Y47" s="10" t="s"/>
+      <x:c r="Z47" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="AA47"/>
+      <x:c r="AB47" s="10" t="s"/>
+      <x:c r="AC47" s="10" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="AD47"/>
+      <x:c r="AE47" s="10" t="s"/>
+      <x:c r="AF47" s="10" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="AG47"/>
+      <x:c r="AH47" s="10" t="s"/>
+      <x:c r="AI47" s="10" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="AJ47"/>
+      <x:c r="AK47" s="10" t="s"/>
+      <x:c r="AL47" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="AM47"/>
+      <x:c r="AN47" s="10" t="s"/>
+      <x:c r="AO47" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="AP47"/>
+      <x:c r="AQ47" s="10" t="s"/>
+      <x:c r="AR47" s="10" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="AS47"/>
+      <x:c r="AT47" s="10" t="s"/>
+      <x:c r="AU47" s="10" t="s"/>
+      <x:c r="AV47"/>
+      <x:c r="AW47" s="10" t="s"/>
+      <x:c r="AX47" s="10" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="AY47"/>
+      <x:c r="AZ47" s="10" t="s"/>
+      <x:c r="BA47" s="10" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="BB47"/>
+      <x:c r="BC47" s="10" t="s"/>
+      <x:c r="BD47" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE47"/>
+      <x:c r="BF47" s="10" t="s"/>
+      <x:c r="BG47" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BH47"/>
+      <x:c r="BI47" s="10" t="s"/>
+      <x:c r="BJ47" s="10" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="BK47"/>
+      <x:c r="BL47" s="10" t="s"/>
+      <x:c r="BM47" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BN47"/>
+      <x:c r="BO47" s="10" t="s"/>
+      <x:c r="BP47" s="10" t="s"/>
+      <x:c r="BQ47"/>
+      <x:c r="BR47" s="10" t="s"/>
+      <x:c r="BS47" s="10" t="s"/>
+      <x:c r="BT47"/>
+      <x:c r="BU47" s="10" t="s"/>
+      <x:c r="BV47" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BW47"/>
+      <x:c r="BX47" s="10" t="s"/>
+      <x:c r="BY47" s="10" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="BZ47"/>
+      <x:c r="CA47" s="10" t="s"/>
+      <x:c r="CB47" s="10" t="s">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="CC47"/>
+      <x:c r="CD47" s="10" t="s"/>
+    </x:row>
+    <x:row r="48" hidden="0">
+      <x:c r="A48">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B48" s="2">
+        <x:v>44174.3516666667</x:v>
+      </x:c>
+      <x:c r="C48" s="2">
+        <x:v>44174.3546875</x:v>
+      </x:c>
+      <x:c r="D48" s="10" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E48" s="10" t="s"/>
+      <x:c r="F48"/>
+      <x:c r="G48" s="10" t="s"/>
+      <x:c r="H48" s="10" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="I48"/>
+      <x:c r="J48" s="10" t="s"/>
+      <x:c r="K48" s="10" t="s">
+        <x:v>392</x:v>
+      </x:c>
+      <x:c r="L48"/>
+      <x:c r="M48" s="10" t="s"/>
+      <x:c r="N48" s="10" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="O48"/>
+      <x:c r="P48" s="10" t="s"/>
+      <x:c r="Q48" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="R48"/>
+      <x:c r="S48" s="10" t="s"/>
+      <x:c r="T48" s="10" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="U48"/>
+      <x:c r="V48" s="10" t="s"/>
+      <x:c r="W48" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="X48"/>
+      <x:c r="Y48" s="10" t="s"/>
+      <x:c r="Z48" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="AA48"/>
+      <x:c r="AB48" s="10" t="s"/>
+      <x:c r="AC48" s="10" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="AD48"/>
+      <x:c r="AE48" s="10" t="s"/>
+      <x:c r="AF48" s="10" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="AG48"/>
+      <x:c r="AH48" s="10" t="s"/>
+      <x:c r="AI48" s="10" t="s">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="AJ48"/>
+      <x:c r="AK48" s="10" t="s"/>
+      <x:c r="AL48" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="AM48"/>
+      <x:c r="AN48" s="10" t="s"/>
+      <x:c r="AO48" s="10" t="s"/>
+      <x:c r="AP48"/>
+      <x:c r="AQ48" s="10" t="s"/>
+      <x:c r="AR48" s="10" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="AS48"/>
+      <x:c r="AT48" s="10" t="s"/>
+      <x:c r="AU48" s="10" t="s"/>
+      <x:c r="AV48"/>
+      <x:c r="AW48" s="10" t="s"/>
+      <x:c r="AX48" s="10" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="AY48"/>
+      <x:c r="AZ48" s="10" t="s"/>
+      <x:c r="BA48" s="10" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="BB48"/>
+      <x:c r="BC48" s="10" t="s"/>
+      <x:c r="BD48" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BE48"/>
+      <x:c r="BF48" s="10" t="s"/>
+      <x:c r="BG48" s="10" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="BH48"/>
+      <x:c r="BI48" s="10" t="s"/>
+      <x:c r="BJ48" s="10" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="BK48"/>
+      <x:c r="BL48" s="10" t="s"/>
+      <x:c r="BM48" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BN48"/>
+      <x:c r="BO48" s="10" t="s"/>
+      <x:c r="BP48" s="10" t="s"/>
+      <x:c r="BQ48"/>
+      <x:c r="BR48" s="10" t="s"/>
+      <x:c r="BS48" s="10" t="s"/>
+      <x:c r="BT48"/>
+      <x:c r="BU48" s="10" t="s"/>
+      <x:c r="BV48" s="10" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="BW48"/>
+      <x:c r="BX48" s="10" t="s"/>
+      <x:c r="BY48" s="10" t="s"/>
+      <x:c r="BZ48"/>
+      <x:c r="CA48" s="10" t="s"/>
+      <x:c r="CB48" s="10" t="s">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="CC48"/>
+      <x:c r="CD48" s="10" t="s"/>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="Ra4d9b6600a7348e9"/>
+    <x:tablePart r:id="Ra63a231f3361469b"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>